<commit_message>
New encyclopedia_table and encyclopedia.db
</commit_message>
<xml_diff>
--- a/atlases/Pan_Immune_CellTypist/encyclopedia/encyclopedia_table.xlsx
+++ b/atlases/Pan_Immune_CellTypist/encyclopedia/encyclopedia_table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="565">
   <si>
     <t>High-hierarchy cell types</t>
   </si>
@@ -37,7 +37,7 @@
     <t>Curated markers</t>
   </si>
   <si>
-    <t>Top 10 important genes from the Celltypist model</t>
+    <t>Top 10 important genes from the CellTypist model</t>
   </si>
   <si>
     <t>B cells</t>
@@ -151,10 +151,10 @@
     <t>Transitional B cells</t>
   </si>
   <si>
-    <t>Immature B cells</t>
-  </si>
-  <si>
-    <t>Pre-B cells</t>
+    <t>Large pre-B cells</t>
+  </si>
+  <si>
+    <t>Small pre-B cells</t>
   </si>
   <si>
     <t>Pre-pro-B cells</t>
@@ -271,18 +271,12 @@
     <t>CD8a/b(entry)</t>
   </si>
   <si>
-    <t>Cytotoxic T cells</t>
-  </si>
-  <si>
     <t>Follicular helper T cells</t>
   </si>
   <si>
     <t>gamma-delta T cells</t>
   </si>
   <si>
-    <t>Helper T cells</t>
-  </si>
-  <si>
     <t>MAIT cells</t>
   </si>
   <si>
@@ -304,7 +298,13 @@
     <t>Tcm/Naive helper T cells</t>
   </si>
   <si>
-    <t>Tem/Effector cytotoxic T cells</t>
+    <t>Tem/Trm cytotoxic T cells</t>
+  </si>
+  <si>
+    <t>Tem/Temra cytotoxic T cells</t>
+  </si>
+  <si>
+    <t>Trm cytotoxic T cells</t>
   </si>
   <si>
     <t>Tem/Effector helper T cells</t>
@@ -340,10 +340,10 @@
     <t>immature B cell precursors in the bone marrow which connect Pre-B cells with mature naive B cells and are subject to the process of B cell selection</t>
   </si>
   <si>
-    <t>immature B cells in the bone marrow expressing IgM on the surface before undergoing immunoglobulin class switching</t>
-  </si>
-  <si>
-    <t>B lymphocyte precursors derived from Pro-B cells and expressing membrane μ chains with surrogate light chains in their receptors</t>
+    <t>proliferative B lymphocyte precursors derived from Pro-B cells and expressing membrane μ chains with surrogate light chains in their receptors</t>
+  </si>
+  <si>
+    <t>non-proliferative B lymphocyte precursors derived from Pro-B cells and expressing membrane μ chains with surrogate light chains in their receptors</t>
   </si>
   <si>
     <t>the earliest primitive B cell progenitors which express CD34 and SPINK2, have germline Ig genes and give rise to Pro-B cells</t>
@@ -541,18 +541,12 @@
     <t>T lymphocytes with CD8 alpha/beta heterodimers in the late double-positive (entry) stage during T cell development</t>
   </si>
   <si>
-    <t>CD8+ T lymphocytes with cytotoxic functions that are specialised for the direct killing of cells that are infected, cancerous or damaged</t>
-  </si>
-  <si>
     <t>specialised CD4+ T cell subpopulation found in the periphery within B cell follicles and stimulating the cognate follicular B cells for class-switching</t>
   </si>
   <si>
     <t>unconventional T lymphocyte subpopulation expressing a gamma-delta T cell receptor complex on the surface to recognise antigens</t>
   </si>
   <si>
-    <t>effector CD4+ T lymphocytes that secrete cytokines and other molecules and help activate other immune cells including B cells and cytotoxic T cells</t>
-  </si>
-  <si>
     <t>mucosal-associated invariant T cells which have semi-invariant T-cell receptors and are restricted by the MHC I-like molecule MR1</t>
   </si>
   <si>
@@ -565,9 +559,6 @@
     <t>T cell subpopulation which modulates immune responses and regulates other cells through direct cell-cell contact and cytokine release</t>
   </si>
   <si>
-    <t>T lymphocytes with T-cell receptors on the cell surface recognising specific antigens and participating in cell-mediated immunity</t>
-  </si>
-  <si>
     <t>unconventional T cell subpopulation in the thymus which expresses MIR155HG and shares some signatures with differentiating regulatory T cells</t>
   </si>
   <si>
@@ -580,6 +571,12 @@
     <t>CD8+ cytotoxic T lymphocytes mainly localized in lymphoid and peripheral tissues and presenting an immediate, but not sustained, immune defense</t>
   </si>
   <si>
+    <t xml:space="preserve">terminally differentiated CD8+ cytotoxic T lymphocytes with effector memory phenotypes that re-express CD45RA </t>
+  </si>
+  <si>
+    <t>tissue resident CD8+ cytotoxic T lymphocytes mainly localized in epithelial tissues such as gut</t>
+  </si>
+  <si>
     <t>CD4+ helper T lymphocytes mainly localized in lymphoid and peripheral tissues and presenting an immediate, but not sustained, immune defense</t>
   </si>
   <si>
@@ -613,9 +610,6 @@
     <t>CL:0000818</t>
   </si>
   <si>
-    <t>CL:0000816</t>
-  </si>
-  <si>
     <t>CL:0000817</t>
   </si>
   <si>
@@ -760,15 +754,9 @@
     <t>CL:0002430</t>
   </si>
   <si>
-    <t>CL:0000910</t>
-  </si>
-  <si>
     <t>CL:0002038</t>
   </si>
   <si>
-    <t>CL:0000912</t>
-  </si>
-  <si>
     <t>CL:0000940</t>
   </si>
   <si>
@@ -790,6 +778,9 @@
     <t>CL:0000913</t>
   </si>
   <si>
+    <t>CL:0001062</t>
+  </si>
+  <si>
     <t>CL:0000905</t>
   </si>
   <si>
@@ -799,79 +790,82 @@
     <t>CL:0000899</t>
   </si>
   <si>
-    <t>Blood, Colon, Decidua, Eye, Intestine, Kidney, Liver, Lung, Spleen, Thymus, Trachea</t>
-  </si>
-  <si>
-    <t>Blood, Colon, Omentum adipose tissue</t>
-  </si>
-  <si>
-    <t>Colon, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Kidney, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen, Thymus</t>
+    <t>Blood, Eye, Intestine, Kidney, Liver, Lung, Thymus, Trachea</t>
+  </si>
+  <si>
+    <t>Colon</t>
+  </si>
+  <si>
+    <t>Colon, Spleen</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Lung, Lung-draining lymph node, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Omentum adipose tissue</t>
+  </si>
+  <si>
+    <t>Bone marrow, Liver, Thymus</t>
+  </si>
+  <si>
+    <t>Bone marrow, Thymus</t>
+  </si>
+  <si>
+    <t>Liver, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Liver, Thymus</t>
+  </si>
+  <si>
+    <t>Spleen</t>
+  </si>
+  <si>
+    <t>Colon, Lung, Spleen</t>
+  </si>
+  <si>
+    <t>Blood, Kidney, Lung, Oesophagus, Omentum adipose tissue, Upper airway</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Liver, Omentum adipose tissue, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Kidney, Liver, Mesenteric lymph node, Omentum adipose tissue, Spleen, Thymus</t>
   </si>
   <si>
     <t>Blood, Bone marrow</t>
   </si>
   <si>
+    <t>Spleen, Thymus</t>
+  </si>
+  <si>
     <t>Blood, Bone marrow, Liver</t>
   </si>
   <si>
-    <t>Liver, Thymus</t>
-  </si>
-  <si>
-    <t>Colon</t>
-  </si>
-  <si>
-    <t>Spleen</t>
-  </si>
-  <si>
-    <t>Colon, Spleen</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Kidney, Lung, Oesophagus, Omentum adipose tissue, Upper airway</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Decidua, Liver, Omentum adipose tissue, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Liver, Mesenteric lymph node, Omentum adipose tissue, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Liver, Omentum adipose tissue</t>
+    <t>Blood, Bone marrow, Omentum adipose tissue, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Omentum adipose tissue, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Oesophagus, Thymus, Trachea, Upper airway</t>
+  </si>
+  <si>
+    <t>Thymus, Trachea</t>
   </si>
   <si>
     <t>Thymus</t>
   </si>
   <si>
-    <t>Omentum adipose tissue, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Thymus</t>
-  </si>
-  <si>
-    <t>Thymus, Trachea</t>
-  </si>
-  <si>
-    <t>Blood, Thymus, Trachea</t>
-  </si>
-  <si>
-    <t>Blood, Liver</t>
-  </si>
-  <si>
-    <t>Blood, Decidua</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Kidney, Omentum adipose tissue, Spleen</t>
-  </si>
-  <si>
-    <t>Blood, Intestine, Liver</t>
+    <t>Blood, Lung, Omentum adipose tissue, Thymus</t>
+  </si>
+  <si>
+    <t>Bone marrow, Decidua</t>
+  </si>
+  <si>
+    <t>Blood, Intestine, Liver, Spleen</t>
   </si>
   <si>
     <t>Bone marrow</t>
@@ -880,25 +874,25 @@
     <t>Liver</t>
   </si>
   <si>
-    <t>Blood, Colon, Intestine, Mesenteric lymph node, Oesophagus, Spleen</t>
-  </si>
-  <si>
-    <t>Omentum adipose tissue, Tonsil</t>
-  </si>
-  <si>
-    <t>Blood, Tonsil</t>
-  </si>
-  <si>
-    <t>Blood, Decidua, Omentum adipose tissue, Thymus, Tonsil</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Decidua, Kidney, Liver, Lung, Mesenteric lymph node, Omentum adipose tissue, Spleen, Thymus, Tonsil</t>
+    <t>Bone marrow, Colon, Intestine, Kidney, Mesenteric lymph node, Oesophagus, Spleen</t>
+  </si>
+  <si>
+    <t>Tonsil</t>
+  </si>
+  <si>
+    <t>Decidua, Lung, Thymus, Tonsil, Trachea</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Kidney, Liver, Lung, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen, Thymus, Tonsil</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Eye, Intestine, Kidney, Liver, Lung, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen, Thymus, Tonsil, Trachea</t>
   </si>
   <si>
     <t>Blood, Bone marrow, Colon, Decidua, Intestine, Kidney, Liver, Lung, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen, Thymus, Tonsil, Trachea</t>
   </si>
   <si>
-    <t>Blood, Bone marrow, Omentum adipose tissue</t>
+    <t>Bone marrow, Omentum adipose tissue</t>
   </si>
   <si>
     <t>Decidua, Placenta</t>
@@ -907,183 +901,198 @@
     <t>Kidney</t>
   </si>
   <si>
-    <t>Blood, Bone marrow, Colon, Decidua, Eye, Intestine, Lung, Mesenteric lymph node, Omentum adipose tissue, Placenta, Spleen, Thymus, Trachea, Upper airway</t>
+    <t>Bone marrow, Colon, Decidua, Eye, Intestine, Lung, Mesenteric lymph node, Omentum adipose tissue, Placenta, Spleen, Thymus, Trachea, Upper airway</t>
   </si>
   <si>
     <t>Bone marrow, Colon, Eye, Intestine, Liver, Lung, Oesophagus, Thymus</t>
   </si>
   <si>
-    <t>Intestine, Omentum adipose tissue</t>
+    <t>Intestine</t>
   </si>
   <si>
     <t>Blood, Bone marrow, Liver, Oesophagus, Omentum adipose tissue, Thymus</t>
   </si>
   <si>
+    <t>Bone marrow, Liver</t>
+  </si>
+  <si>
     <t>Blood, Bone marrow, Colon, Kidney, Liver, Lung, Omentum adipose tissue, Spleen, Thymus, Upper airway</t>
   </si>
   <si>
     <t>Blood, Bone marrow, Colon, Decidua, Kidney, Liver, Lung, Omentum adipose tissue, Spleen, Thymus, Upper airway</t>
   </si>
   <si>
+    <t>Blood, Bone marrow, Colon, Lung, Omentum adipose tissue</t>
+  </si>
+  <si>
     <t>Blood, Bone marrow, Decidua, Kidney, Lung, Spleen, Thymus</t>
   </si>
   <si>
-    <t>Blood, Bone marrow, Colon, Intestine, Lung, Mesenteric lymph node, Omentum adipose tissue, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Decidua, Kidney, Lung, Lung-draining lymph node, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen, Thymus, Upper airway</t>
-  </si>
-  <si>
-    <t>Colon, Mesenteric lymph node, Spleen, Thymus</t>
+    <t>Blood, Bone marrow, Colon, Intestine, Kidney, Lung, Lung-draining lymph node, Mesenteric lymph node, Omentum adipose tissue, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Intestine, Lung, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Lung, Lung-draining lymph node, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Intestine, Kidney, Lung-draining lymph node, Mesenteric lymph node, Oesophagus, Spleen, Thymus</t>
   </si>
   <si>
     <t>Colon, Mesenteric lymph node</t>
   </si>
   <si>
-    <t>Blood, Bone marrow, Colon, Decidua, Intestine, Kidney, Lung, Lung-draining lymph node, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Skin, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Decidua, Spleen</t>
-  </si>
-  <si>
-    <t>Blood, Kidney, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Decidua, Intestine, Mesenteric lymph node, Skin, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Eye, Intestine, Kidney, Lung, Omentum adipose tissue, Spleen, Thymus, Trachea, Upper airway</t>
-  </si>
-  <si>
-    <t>Blood, Intestine, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Decidua, Mesenteric lymph node, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Decidua, Intestine, Mesenteric lymph node, Omentum adipose tissue, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Eye, Kidney, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Omentum adipose tissue, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Omentum adipose tissue, Thymus</t>
-  </si>
-  <si>
-    <t>Bone marrow, Colon, Mesenteric lymph node, Omentum adipose tissue</t>
-  </si>
-  <si>
-    <t>Blood, Colon, Intestine, Mesenteric lymph node, Thymus</t>
-  </si>
-  <si>
-    <t>Braga et al. 2019, HCA Immune 2018, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Miller et al. 2020, Park et al. 2020, Popescu et al. 2019, Stewart et al. 2019, Vento-Tormo et al. 2018, Voigt et al. 2019, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Jaitin et al. 2019, Smillie et al. 2019</t>
-  </si>
-  <si>
-    <t>James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Smillie et al. 2019</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Stewart et al. 2019</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020</t>
+    <t>Blood, Bone marrow, Colon, Decidua, Intestine, Kidney, Mesenteric lymph node, Oesophagus, Spleen</t>
+  </si>
+  <si>
+    <t>Bone marrow, Kidney, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Intestine, Kidney, Lung, Lung-draining lymph node, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Skin, Spleen, Thymus, Trachea</t>
+  </si>
+  <si>
+    <t>Intestine, Thymus, Trachea</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Intestine, Kidney, Lung, Lung-draining lymph node, Mesenteric lymph node, Oesophagus, Spleen, Thymus, Trachea</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Intestine, Kidney, Lung, Lung-draining lymph node, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen, Thymus, Trachea</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Eye, Intestine, Kidney, Lung, Lung-draining lymph node, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Eye, Lung, Lung-draining lymph node, Oesophagus, Omentum adipose tissue, Spleen</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Intestine, Kidney, Lung, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Intestine, Kidney, Lung, Lung-draining lymph node, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen, Thymus, Upper airway</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Intestine, Kidney, Lung, Lung-draining lymph node, Mesenteric lymph node, Spleen, Thymus, Trachea</t>
+  </si>
+  <si>
+    <t>Bone marrow, Colon, Decidua, Intestine, Kidney, Lung, Mesenteric lymph node, Spleen</t>
+  </si>
+  <si>
+    <t>Blood, Colon, Decidua, Intestine, Kidney, Lung, Lung-draining lymph node, Mesenteric lymph node, Oesophagus, Spleen, Thymus, Trachea</t>
+  </si>
+  <si>
+    <t>Braga et al. 2019, HCA Immune 2018, Martin et al. 2019, Miller et al. 2020, Park et al. 2020, Popescu et al. 2019, Stewart et al. 2019, Voigt et al. 2019, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>Smillie et al. 2019</t>
+  </si>
+  <si>
+    <t>James et al. 2020, Madissoon et al. 2020, Smillie et al. 2019</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Szabo et al. 2019, Vento-Tormo et al. 2018</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Park et al. 2020, Popescu et al. 2019</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Park et al. 2020</t>
+  </si>
+  <si>
+    <t>Park et al. 2020, Popescu et al. 2019</t>
+  </si>
+  <si>
+    <t>James et al. 2020, Smillie et al. 2019</t>
+  </si>
+  <si>
+    <t>James et al. 2020</t>
+  </si>
+  <si>
+    <t>Madissoon et al. 2020</t>
+  </si>
+  <si>
+    <t>Braga et al. 2019, Madissoon et al. 2020, Smillie et al. 2019</t>
+  </si>
+  <si>
+    <t>Braga et al. 2019, Jaitin et al. 2019, Madissoon et al. 2020, Stewart et al. 2019, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Vento-Tormo et al. 2018</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Stewart et al. 2019, Vento-Tormo et al. 2018</t>
   </si>
   <si>
     <t>HCA Immune 2018</t>
   </si>
   <si>
+    <t>Madissoon et al. 2020, Park et al. 2020</t>
+  </si>
+  <si>
     <t>HCA Immune 2018, Popescu et al. 2019</t>
   </si>
   <si>
-    <t>Park et al. 2020, Popescu et al. 2019</t>
-  </si>
-  <si>
-    <t>James et al. 2020, Smillie et al. 2019</t>
-  </si>
-  <si>
-    <t>James et al. 2020</t>
-  </si>
-  <si>
-    <t>Smillie et al. 2019</t>
-  </si>
-  <si>
-    <t>Madissoon et al. 2020</t>
-  </si>
-  <si>
-    <t>Madissoon et al. 2020, Smillie et al. 2019</t>
-  </si>
-  <si>
-    <t>Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, Madissoon et al. 2020, Stewart et al. 2019, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Vento-Tormo et al. 2018</t>
-  </si>
-  <si>
-    <t>Madissoon et al. 2020, Park et al. 2020</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Jaitin et al. 2019, Popescu et al. 2019</t>
+    <t>HCA Immune 2018, Jaitin et al. 2019, Madissoon et al. 2020, Park et al. 2020</t>
+  </si>
+  <si>
+    <t>Jaitin et al. 2019, Park et al. 2020, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>Braga et al. 2019, Madissoon et al. 2020, Miller et al. 2020, Park et al. 2020, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>Miller et al. 2020, Park et al. 2020</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Popescu et al. 2019, Zheng et al. 2017</t>
   </si>
   <si>
     <t>Park et al. 2020</t>
   </si>
   <si>
-    <t>Jaitin et al. 2019, Park et al. 2020</t>
-  </si>
-  <si>
-    <t>Park et al. 2020, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>Miller et al. 2020, Park et al. 2020</t>
-  </si>
-  <si>
-    <t>Miller et al. 2020, Park et al. 2020, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Popescu et al. 2019, Zheng et al. 2017</t>
+    <t>Jaitin et al. 2019, Miller et al. 2020, Park et al. 2020, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Vento-Tormo et al. 2018</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Li et al. 2019, Madissoon et al. 2020, Popescu et al. 2019</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Popescu et al. 2019, Vento-Tormo et al. 2018</t>
+  </si>
+  <si>
+    <t>Popescu et al. 2019</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Smillie et al. 2019, Stewart et al. 2019</t>
+  </si>
+  <si>
+    <t>Bjorklund et al. 2016</t>
+  </si>
+  <si>
+    <t>Bjorklund et al. 2016, Miller et al. 2020, Park et al. 2020, Vento-Tormo et al. 2018</t>
+  </si>
+  <si>
+    <t>Bjorklund et al. 2016, Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Miller et al. 2020, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Stewart et al. 2019, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>Bjorklund et al. 2016, Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Li et al. 2019, Madissoon et al. 2020, Martin et al. 2019, Miller et al. 2020, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Stewart et al. 2019, Vento-Tormo et al. 2018, Voigt et al. 2019, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>Bjorklund et al. 2016, Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Miller et al. 2020, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Stewart et al. 2019, Szabo et al. 2019, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
   </si>
   <si>
     <t>Vento-Tormo et al. 2018</t>
   </si>
   <si>
-    <t>HCA Immune 2018, Jaitin et al. 2019, Madissoon et al. 2020, Stewart et al. 2019</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Li et al. 2019, Popescu et al. 2019</t>
-  </si>
-  <si>
-    <t>Popescu et al. 2019</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Smillie et al. 2019</t>
-  </si>
-  <si>
-    <t>Bjorklund et al. 2016, Jaitin et al. 2019</t>
-  </si>
-  <si>
-    <t>Bjorklund et al. 2016, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>Bjorklund et al. 2016, Jaitin et al. 2019, Park et al. 2020, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>Bjorklund et al. 2016, Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Miller et al. 2020, Park et al. 2020, Popescu et al. 2019, Stewart et al. 2019, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>Bjorklund et al. 2016, Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Miller et al. 2020, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Stewart et al. 2019, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Jaitin et al. 2019</t>
-  </si>
-  <si>
     <t>Stewart et al. 2019</t>
   </si>
   <si>
@@ -1093,7 +1102,7 @@
     <t>Braga et al. 2019, HCA Immune 2018, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Voigt et al. 2019</t>
   </si>
   <si>
-    <t>Jaitin et al. 2019, Martin et al. 2019</t>
+    <t>Martin et al. 2019</t>
   </si>
   <si>
     <t>HCA Immune 2018, Jaitin et al. 2019, Madissoon et al. 2020, Park et al. 2020, Popescu et al. 2019</t>
@@ -1102,61 +1111,64 @@
     <t>Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Popescu et al. 2019, Stewart et al. 2019, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
   </si>
   <si>
-    <t>Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Stewart et al. 2019, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
+    <t>Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Popescu et al. 2019, Stewart et al. 2019, Szabo et al. 2019, Vento-Tormo et al. 2018</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, Smillie et al. 2019, Szabo et al. 2019</t>
   </si>
   <si>
     <t>Braga et al. 2019, HCA Immune 2018, Madissoon et al. 2020, Park et al. 2020, Stewart et al. 2019, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
   </si>
   <si>
-    <t>Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Park et al. 2020, Smillie et al. 2019, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Madissoon et al. 2020, Park et al. 2020, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Smillie et al. 2019, Stewart et al. 2019, Szabo et al. 2019, Vento-Tormo et al. 2018, Zhang et al. 2018, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>James et al. 2020, Madissoon et al. 2020, Park et al. 2020</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Li et al. 2019, Madissoon et al. 2020, Martin et al. 2019, Miragaia et al. 2019, Park et al. 2020, Smillie et al. 2019, Stewart et al. 2019, Szabo et al. 2019, Vento-Tormo et al. 2018, Zhang et al. 2018, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Madissoon et al. 2020, Vento-Tormo et al. 2018</t>
-  </si>
-  <si>
-    <t>Park et al. 2020, Stewart et al. 2019, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, James et al. 2020, Li et al. 2019, Madissoon et al. 2020, Miragaia et al. 2019, Park et al. 2020, Smillie et al. 2019, Vento-Tormo et al. 2018, Zhang et al. 2018, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, Li et al. 2019, Madissoon et al. 2020, Martin et al. 2019, Miller et al. 2020, Park et al. 2020, Stewart et al. 2019, Voigt et al. 2019</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Li et al. 2019, Park et al. 2020</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Vento-Tormo et al. 2018, Zhang et al. 2018, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Li et al. 2019, Madissoon et al. 2020, Park et al. 2020, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>Madissoon et al. 2020, Park et al. 2020, Stewart et al. 2019, Voigt et al. 2019, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Jaitin et al. 2019, Park et al. 2020, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Jaitin et al. 2019, Park et al. 2020</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, James et al. 2020, Li et al. 2019, Park et al. 2020</t>
+    <t>Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Park et al. 2020, Smillie et al. 2019, Stewart et al. 2019, Szabo et al. 2019, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Madissoon et al. 2020, Martin et al. 2019, Park et al. 2020, Szabo et al. 2019</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Park et al. 2020, Szabo et al. 2019</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, James et al. 2020, Li et al. 2019, Madissoon et al. 2020, Martin et al. 2019, Park et al. 2020, Stewart et al. 2019, Szabo et al. 2019, Vento-Tormo et al. 2018</t>
+  </si>
+  <si>
+    <t>James et al. 2020, Smillie et al. 2019, Zhang et al. 2018</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Smillie et al. 2019, Stewart et al. 2019, Vento-Tormo et al. 2018, Zhang et al. 2018, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Park et al. 2020, Stewart et al. 2019</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Li et al. 2019, Madissoon et al. 2020, Martin et al. 2019, Miller et al. 2020, Miragaia et al. 2019, Park et al. 2020, Smillie et al. 2019, Stewart et al. 2019, Szabo et al. 2019, Vento-Tormo et al. 2018, Zhang et al. 2018, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>Li et al. 2019, Miller et al. 2020, Park et al. 2020</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Miller et al. 2020, Park et al. 2020, Smillie et al. 2019, Stewart et al. 2019, Szabo et al. 2019, Vento-Tormo et al. 2018, Zhang et al. 2018, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Park et al. 2020, Smillie et al. 2019, Stewart et al. 2019, Szabo et al. 2019, Vento-Tormo et al. 2018, Voigt et al. 2019, Zhang et al. 2018, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, Madissoon et al. 2020, Szabo et al. 2019, Vento-Tormo et al. 2018, Voigt et al. 2019, Zhang et al. 2018</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Smillie et al. 2019, Stewart et al. 2019, Szabo et al. 2019, Zhang et al. 2018</t>
+  </si>
+  <si>
+    <t>Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Park et al. 2020, Smillie et al. 2019, Stewart et al. 2019, Szabo et al. 2019, Vento-Tormo et al. 2018, Zhang et al. 2018, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Miller et al. 2020, Park et al. 2020, Stewart et al. 2019, Szabo et al. 2019</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, James et al. 2020, Li et al. 2019, Madissoon et al. 2020, Martin et al. 2019, Smillie et al. 2019, Stewart et al. 2019, Szabo et al. 2019, Vento-Tormo et al. 2018, Zhang et al. 2018</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, James et al. 2020, Li et al. 2019, Madissoon et al. 2020, Martin et al. 2019, Miller et al. 2020, Park et al. 2020, Smillie et al. 2019, Stewart et al. 2019, Szabo et al. 2019, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
   </si>
   <si>
     <t>CD79A, MS4A1, CD19</t>
@@ -1177,16 +1189,16 @@
     <t>CD24, MYO1C, MS4A1</t>
   </si>
   <si>
-    <t>IGHM, CD24, IGLL5</t>
-  </si>
-  <si>
-    <t>MME, CD24, IGLL1</t>
-  </si>
-  <si>
-    <t>CD22, ZCCHC7, CD24</t>
-  </si>
-  <si>
-    <t>CD22, DNTT, IGLL1</t>
+    <t>MME, CD24, MKI67</t>
+  </si>
+  <si>
+    <t>MME, CD24, IGLL5</t>
+  </si>
+  <si>
+    <t>IL7R, ZCCHC7, RAG1</t>
+  </si>
+  <si>
+    <t>MME, DNTT, IGLL1</t>
   </si>
   <si>
     <t>MKI67, TOP2A, CD19</t>
@@ -1246,13 +1258,13 @@
     <t>HBM, HBQ1, GYPA</t>
   </si>
   <si>
-    <t>APOC1, KLF1, GATA2</t>
+    <t>APOC1, TESPA1, GATA2</t>
   </si>
   <si>
     <t>GYPA, GYPB, HBA1</t>
   </si>
   <si>
-    <t>KLF1, KCNH2, HBG1</t>
+    <t>PRDX2, KCNH2, GYPA</t>
   </si>
   <si>
     <t>ACY3, SPINK2, CD34</t>
@@ -1264,16 +1276,16 @@
     <t>KIT, CPA3, SLC45A3</t>
   </si>
   <si>
-    <t>S100A9, NAMPT, G0S2</t>
-  </si>
-  <si>
-    <t>SPINK2, CTSG, FLT3</t>
-  </si>
-  <si>
-    <t>ETS1, RIPOR2, GATA3</t>
-  </si>
-  <si>
-    <t>FLT3, SPINK2, RUNX2</t>
+    <t>LCN2, ORM1, MMP8</t>
+  </si>
+  <si>
+    <t>MPO, CTSG, FLT3</t>
+  </si>
+  <si>
+    <t>ETS1, IL32, GATA3</t>
+  </si>
+  <si>
+    <t>FLT3, LTB, RUNX2</t>
   </si>
   <si>
     <t>ELANE, MPO, PRTN3</t>
@@ -1282,13 +1294,13 @@
     <t>CD34, SPINK2, CRHBP</t>
   </si>
   <si>
-    <t>GATA2, FCER1A, PRSS57</t>
-  </si>
-  <si>
-    <t>GATA2, ITGA2B, PRSS57</t>
-  </si>
-  <si>
-    <t>SPINK2, MPO, CD34</t>
+    <t>GATA2, FCER1A, GATA1</t>
+  </si>
+  <si>
+    <t>GATA2, ITGA2B, GATA1</t>
+  </si>
+  <si>
+    <t>LYZ, MPO, SERPINB1</t>
   </si>
   <si>
     <t>S100A13, TLE1, AREG</t>
@@ -1300,7 +1312,7 @@
     <t>GATA3, KLRG1, HPGDS</t>
   </si>
   <si>
-    <t>IL4I1, RORC, IL7R</t>
+    <t>IL4I1, RORC, KIT</t>
   </si>
   <si>
     <t>GNLY, FCGR3A, NKG7</t>
@@ -1315,7 +1327,7 @@
     <t>CCL5, GZMK, FCGR3A</t>
   </si>
   <si>
-    <t>LST1, KIT, SCN1B</t>
+    <t>LST1, HPN, SCN1B</t>
   </si>
   <si>
     <t>LYVE1, SCIN, F13A1</t>
@@ -1378,18 +1390,12 @@
     <t>TOX2, SATB1, CCR9</t>
   </si>
   <si>
-    <t>NKG7, CD8A, CCL5</t>
-  </si>
-  <si>
     <t>PDCD1, ICOS, CXCR5</t>
   </si>
   <si>
     <t>TRDC, TRGC1, CCL5</t>
   </si>
   <si>
-    <t>IL7R, IL32, CD4</t>
-  </si>
-  <si>
     <t>KLRB1, SLC4A10, TRAV1-2</t>
   </si>
   <si>
@@ -1402,9 +1408,6 @@
     <t>CTLA4, IL2RA, FOXP3</t>
   </si>
   <si>
-    <t>CD3D, CD3G, CD3E</t>
-  </si>
-  <si>
     <t>MIR155HG, BIRC3, SMS</t>
   </si>
   <si>
@@ -1414,10 +1417,16 @@
     <t>CCR7, SELL, CD4</t>
   </si>
   <si>
-    <t>GZMK, CD8A, NKG7</t>
-  </si>
-  <si>
-    <t>IL32, SELL, CD4</t>
+    <t>GZMK, CD8A, CCL5</t>
+  </si>
+  <si>
+    <t>CX3CR1, GZMB, GNLY</t>
+  </si>
+  <si>
+    <t>ITGA1, ITGAE, CXCR6</t>
+  </si>
+  <si>
+    <t>KLRB1, AQP3, ITGB1</t>
   </si>
   <si>
     <t>PDCD1, CD4, CTLA4</t>
@@ -1432,277 +1441,274 @@
     <t>IL7R, CCR6, ZBTB16</t>
   </si>
   <si>
-    <t>RACK1, HSPA1B, PTMA, HBG2, CD79A, HLA-DRB1, RPL10, MALAT1, ATP5F1E, HLA-DRA</t>
-  </si>
-  <si>
-    <t>MT-RNR2, RPL41, CD74, IGHA1, CXCR4, HLA-DRA, H3F3A, CD83, VPREB3, FTH1</t>
-  </si>
-  <si>
-    <t>KIAA0101, TCL1A, MS4A1, CELF2-AS2, RPS15A, OCM, FIGF, BCAN, AC245060.6, AL627171.2</t>
-  </si>
-  <si>
-    <t>HLA-DRA, MALAT1, MIR1244-2, RPS17, CD74, MT-ATP8, MT-ND4L, RPL39, HES1, RPL41</t>
-  </si>
-  <si>
-    <t>GNB2L1, IGHD, TCL1A, AL450405.1, YBX3, IGHM, CD74, PTPRC, ATP5E, IL4R</t>
-  </si>
-  <si>
-    <t>MIR1244-2, RPS24, CD79A, H3F3B, IGHM, TMSB10, PTMA, RPSAP15, ERICH5, RPL10P9</t>
-  </si>
-  <si>
-    <t>CD79B, PTMA, MIR1244-2, IGHM, CELF2-AS2, GBP7, AC020915.1, BCAN, SOX4, RPL21P134</t>
-  </si>
-  <si>
-    <t>IGLL1, TCL1A, PCLAF, VPREB1, PDLIM1, AC135507.1, RPSAP15, VAT1L, RP4-665J23.1, IER3-AS1</t>
-  </si>
-  <si>
-    <t>VPREB1, JCHAIN, IGLL1, LST1, RPSAP15, UHRF1, KIAA0226L, PTMA, RNU6-540P, MN1</t>
-  </si>
-  <si>
-    <t>DNTT, VPREB1, VPREB3, IGLL1, AC072061.1, RPSAP15, FTH1P20, AKAP12, AL021937.2, OR11G2</t>
-  </si>
-  <si>
-    <t>AC023590.1, RPSAP15, EFNB3, SAMMSON, DIO3OS, NDUFA6-DT, TCL1A, FTH1, RP11-736K20.5, RNU7-18P</t>
-  </si>
-  <si>
-    <t>RPSAP15, TMEM132C, MIR7111, SDS, AC005253.1, RNU6-151P, PRR16, AC107032.1, RNVU1-7, RPL7P52</t>
-  </si>
-  <si>
-    <t>RPSAP15, CELF2-AS2, HSPC324, TRBJ2-3, AL161781.2, OR11G2, AC004967.7, AC079610.2, PRR16, LINC00892</t>
-  </si>
-  <si>
-    <t>PCLAF, RPSAP15, AJ271736.10, MYOC, AP000936.1, AC107032.1, AL021937.2, TK1, AC090602.2, RNU6-540P</t>
-  </si>
-  <si>
-    <t>KIAA0101, STMN1, TUBA1B, TYMS, NKG7, ASPM, IGKC, HMGB2, HSPC324, CD38</t>
-  </si>
-  <si>
-    <t>STMN1, KIAA0101, IL32, ASPM, HMGB2, RRM2, RPSAP15, MT-CO3, TRBV28, SNORA67</t>
-  </si>
-  <si>
-    <t>RGS1, LYZ, HLA-DQA1, GPX1, HLA-DQB1, ENHO, CXCL10, FCER1A, CCL17, AL161781.2</t>
-  </si>
-  <si>
-    <t>C1orf54, LYZ, IRF8, RAB7B, WFDC21P, CPVL, RPSAP15, SNORA70, OR11G2, CHMP4BP1</t>
-  </si>
-  <si>
-    <t>RPL41, CLEC10A, JAML, H3F3A, RPL39, HLA-DQB1, EEF1A1, CST3, HLA-DRB5, HSPB1</t>
-  </si>
-  <si>
-    <t>LMNA, FCN1, RPSAP15, FMO2, PTMA, FCER1A, PRNCR1, POC1B-AS1, AC004967.7, SHISA3</t>
-  </si>
-  <si>
-    <t>NCCRP1, CCL19, TNFRSF11B, EBI3, RPSAP15, WNT5B, AC107032.1, RNU6-540P, SNORA70, HSPC324</t>
-  </si>
-  <si>
-    <t>PPM1J, HLA-DPB2, CXCL8, AXL, AL021937.2, PSMD6-AS1, RNU6-450P, SHISA3, RPSAP15, AL096870.2</t>
-  </si>
-  <si>
-    <t>PCLAF, CST3, RNASE2, RPSAP15, LY6E-DT, TRBV28, HLA-DRB6, TMSB10, LYZ, AL161781.2</t>
-  </si>
-  <si>
-    <t>CD99, PTCRA, IGLL1, FXYD2, MZB1, JCHAIN, RP11-620J15.3, PDLIM1, ADA, TMSB10</t>
-  </si>
-  <si>
-    <t>SMPD3, CD1B, SH3TC1, CD8B, CD1E, TCF7, TRDC, TRBC2, ELOVL4, CD8A</t>
-  </si>
-  <si>
-    <t>WFDC1, DNM3, GP1BA, MED12L, SLC18A2, SELP, RPSAP15, HSPC324, TBXA2R, OR11G2</t>
-  </si>
-  <si>
-    <t>ACKR1, RAMP3, PLVAP, CX3CL1, NRN1, SDPR, ZNF385D, MYRIP, HOXD8, TSPAN12</t>
-  </si>
-  <si>
-    <t>WFDC2, FRMD1, TOX3, FOXC1, CDH3, NXN, FAM150B, PNCK, IGDCC3, CDC42EP5</t>
-  </si>
-  <si>
-    <t>HBG2, RPSAP15, MYOC, PNMT, HBZ, FAM65C, AC004967.7, CH17-472G23.2, RPS2P44, SERPINB10</t>
-  </si>
-  <si>
-    <t>ERFE, FAM178B, HBB, RNF182, AFP, PCLAF, GAD1, AC106795.1, PRG2, RP4-717I23.3</t>
-  </si>
-  <si>
-    <t>RPSAP15, RP11-465B22.3, HMGCLL1, AL109767.1, AP000580.1, AL157938.1, HRCT1, CH17-472G23.2, HBA1, RP11-736K20.5</t>
-  </si>
-  <si>
-    <t>FAM178B, RPS4Y1, RPSAP15, PCLAF, SYNGR1, TMCC2, GIHCG, MAMLD1, BLVRB, AL592494.3</t>
-  </si>
-  <si>
-    <t>ACY3, SPINK2, KIAA0125, RP11-163E9.1, RPSAP15, AC096664.2, AC093635.1, INSL3, PRDM16, AC009041.2</t>
-  </si>
-  <si>
-    <t>NTRK2, SMOC2, SFRP1, OLFML1, PRRX1, SCARA5, RSPO3, ANGPTL1, NRK, ISLR</t>
-  </si>
-  <si>
-    <t>AL157895.1, MAMDC2, AC008781.2, AC026471.4, AL450384.2, AC004967.7, TPSB2, HSPC324, PAGE4, RPSAP15</t>
-  </si>
-  <si>
-    <t>PTPRC, LYZ, FTL, FTH1, S100A8, MT-RNR2, DEFA1, RPSAP15, MYOC, MT-RNR1</t>
-  </si>
-  <si>
-    <t>SPINK2, AC108866.1, LINC01786, RPL10P2, LINC01694, C1QTNF4, EEF1DP7, RPSAP15, AC092597.1, MIR4453HG</t>
-  </si>
-  <si>
-    <t>HBG2, HBA2, ATP5F1E, RACK1, IL32, HBA1, PTPRC, CST3, RPS17, H3F3A</t>
-  </si>
-  <si>
-    <t>AL096865.1, TRBV28, OSGEPL1-AS1, RNU6-450P, SPINK2, SSSCA1-AS1, RPSAP15, FAM30A, FALEC, ZNF280B</t>
-  </si>
-  <si>
-    <t>ELANE, SERPINB10, C1QTNF4, RPSAP15, HCG4P5, SNORA70, MPO, HOXA5, ZNF792, OR11G2</t>
-  </si>
-  <si>
-    <t>SPINK2, HOPX, RNU7-18P, MDK, LINC01011, AC007098.1, CD34, BEX3, AC007032.1, SERPINB10</t>
-  </si>
-  <si>
-    <t>GP9, CKB, FCER1A, PCLAF, CMTM5, RP11-357H14.17, CELF2-AS2, RP1-79C4.4, RPSAP15, AC107032.1</t>
-  </si>
-  <si>
-    <t>GIHCG, PRSS57, ITGA2B, CNRIP1, TPSAB1, EEF1A1P9, TMOD1, Z98884.1, AL691447.2, EML2-AS1</t>
-  </si>
-  <si>
-    <t>MPO, HIST1H1D, PRSS57, RPSAP15, PRTN3, RNU6-540P, AC104806.2, AL139246.3, AC009041.2, AC104563.1</t>
-  </si>
-  <si>
-    <t>AREG, IL7R, LST1, CSF2, TYROBP, MALAT1, S100A13, TNFSF13B, IGHA1, AC017002.1</t>
-  </si>
-  <si>
-    <t>RPS29P16, MTND4P12, RPS12P26, RPL23AP18, RPS3P6, RPL19P12, EIF1P3, RP4-665J23.1, MYOC, RPL37AP8</t>
-  </si>
-  <si>
-    <t>KRT1, MTCO3P12, MTND4P12, SLITRK2, RPSAP15, AC104563.1, TMEM132C, RPS2P44, CELF2-AS2, A2MP1</t>
-  </si>
-  <si>
-    <t>IL7R, TRDC, LINC00299, SLITRK2, TOX2, RPSAP15, CTSW, AC090948.3, XCL1, SPINK2</t>
-  </si>
-  <si>
-    <t>FCER1G, GNLY, TYROBP, IGFBP7, GZMB, MYOM2, PTGDS, LINC00299, FCGR3A, ADAMTS1</t>
-  </si>
-  <si>
-    <t>TYROBP, LDB2, CCL3, NKG7, FCER1G, GSTP1, KLRB1, CLIC3, IRF8, CXCL3</t>
-  </si>
-  <si>
-    <t>NKG7, CST3, GNLY, SPINK2, CDC20, RP11-445P19.3, HBG2, GPR56, IGFBP4, TTLL10</t>
-  </si>
-  <si>
-    <t>GNLY, TYROBP, IFITM2, H3F3B, CMC1, RPSAP15, MIR1244-2, KLRB1, STX17-AS1, MYOC</t>
-  </si>
-  <si>
-    <t>LST1, RBM24, HSPB1, NMU, HBA2, RPSAP15, AC016596.1, IL1A, RPS15A, CORO2B</t>
-  </si>
-  <si>
-    <t>PAGE4, CGA, LYVE1, METTL7B, SLC28A1, XAGE3, RPSAP15, AC090948.3, AC012085.2, AL513550.1</t>
-  </si>
-  <si>
-    <t>SEPP1, RPSAP15, RNU6-540P, AC007032.1, AL021937.2, AL592494.3, HMGCLL1, GATA6-AS1, ALOX15P1, LGR6</t>
-  </si>
-  <si>
-    <t>HBA2, CETP, HBG2, SNORD3D, TMSB10, HBA1, VCAM1, TMSB4X, EPB41L2, FTH1</t>
-  </si>
-  <si>
-    <t>GNLY, SEPP1, KIAA1598, IL8, CD5L, FTH1, FTL, AMICA1, APOE, C1QA</t>
-  </si>
-  <si>
-    <t>CPA3, TPSAB1, FTH1, PRG2, HPGDS, MYOC, RPSAP15, RP13-93L13.2, SLC18A2, RPS3AP12</t>
-  </si>
-  <si>
-    <t>FCER1A, VSTM1, LINC02573, HMGCLL1, AL356535.1, RNVU1-7, CYTL1, RPL19P12, TMEM132C, PRR16</t>
-  </si>
-  <si>
-    <t>RPSAP15, MYEOV, ESAM, OR11G2, HSPC324, AL021937.2, GPR150, RP13-93L13.2, C12orf42, CELF2-AS2</t>
-  </si>
-  <si>
-    <t>CST3, RPSAP15, FAM26F, CEBPD, IFI30, PTMA, MTRNR2L10, AC079610.2, SEPP1, MT-CO3</t>
-  </si>
-  <si>
-    <t>KLRB1, NKG7, C1QC, HLA-DRA, GPX1, FTH1, HBG2, SPRR3, KRT13, C1orf226</t>
-  </si>
-  <si>
-    <t>RETN, HBG2, LYZ, S100A8, FCN1, H3F3A, CRHR1-IT1, RPSAP15, RAB5IF, RP4-717I23.3</t>
-  </si>
-  <si>
-    <t>S100A9, ATP5E, FTL, NEAT1, TYROBP, HBG2, EEF1A1, CST3, MT-CO1, RPL7</t>
-  </si>
-  <si>
-    <t>RHOC, DNAJA4, HES4, HSPH1, HSPB1, MT2A, ABI3, CD52, MS4A7, ACTB</t>
-  </si>
-  <si>
-    <t>TYROBP, FTL, LYZ, NEAT1, HLA-DPB1, AL450405.1, AC090498.1, CYP4F3, AL355388.1, KIAA0101</t>
-  </si>
-  <si>
-    <t>FTH1, LYZ, FTL, S100A6, TYROBP, SRGN, PTPRC, MT-ND3, CROCC2, CST3</t>
-  </si>
-  <si>
-    <t>AL357143.1, PLD4, CACNB4, IRF8, GZMB, AC023590.1, JCHAIN, AC119428.2, AC098613.1, FTH1</t>
-  </si>
-  <si>
-    <t>TPM2, RPSAP15, TNNI2, IL3RA, SSTR3, RP4-665J23.1, PTPRR, LY6E-DT, AL161781.2, BTNL8</t>
-  </si>
-  <si>
-    <t>JCHAIN, MZB1, XBP1, HSP90B1, IGKC, IGHA2, TSPAN8, ITGA6-AS1, ELFN1-AS1, RPSAP15</t>
-  </si>
-  <si>
-    <t>PTMA, CFD, PCLAF, RP11-357H14.17, CLEC12B, LYZ, CITED1, SLC44A1, AC137630.3, RPSAP15</t>
-  </si>
-  <si>
-    <t>NUCB2, CD27, GAPDH, MALAT1, LEF1, VIM, CD8A, PRKCH, ZNF683, GNG4</t>
-  </si>
-  <si>
-    <t>MALAT1, ITM2A, CD1E, RPL10, SATB1, HSPH1, RPS27, FYB, FTL, TMSB10</t>
-  </si>
-  <si>
-    <t>CCL5, SERPINF1, CD8B, NKG7, CD8A, SOX4, KRT13, RP11-466H18.1, S100B, MT-RNR2</t>
-  </si>
-  <si>
-    <t>SOCS3, KLRB1, MALAT1, CH25H, PVALB, SRGN, ICOS, HMGCLL1, TRBV28, CELF2-AS2</t>
-  </si>
-  <si>
-    <t>KIR2DL4, KLRC2, LAYN, MYOC, IL1A, ASB15, SERPINB10, TRDC, LINC01635, DRAIC</t>
-  </si>
-  <si>
-    <t>RPL41, SYT14, GNB2L1, EEF1A1, GAS5, HLA-H, MT-RNR2, GLTSCR2, SPP1, RPS29</t>
-  </si>
-  <si>
-    <t>KLRB1, CEBPD, IL7R, GZMK, KLRG1, AC090498.1, RPS17, PRF1, SLC4A10, MT-ND3</t>
-  </si>
-  <si>
-    <t>GZMK, GZMA, DNTT, DONSON, RPSAP15, AL590822.2, YY2, AC007032.1, AC096733.2, MIR3188</t>
-  </si>
-  <si>
-    <t>NKG7, AIF1, GNLY, ITM2C, CD52, LDB2, HSPA1B, GZMH, PRDM16, RPL39</t>
-  </si>
-  <si>
-    <t>MS4A6A, IL32, TIMD4, SRGN, FTL, MIR3188, HLA-A, LINC00299, RTKN2, RPS27</t>
-  </si>
-  <si>
-    <t>RPS17, FCGR3A, MALAT1, RGS1, RPL39, SCGB3A2, KLRD1, TMEM66, CCL5, B2M</t>
-  </si>
-  <si>
-    <t>GAPDH, HLA-B, SMS, PKM, CD74, PTMA, TUBB, PTPRC, BIRC3, COTL1</t>
-  </si>
-  <si>
-    <t>CD8B, CD8A, RPS2, B2M, LINC02446, GNB2L1, HLA-B, HSPH1, RPL13, FTL</t>
-  </si>
-  <si>
-    <t>AL450405.1, MT-RNR2, EEF1A1, CTSL, IGLL5, TMSB10, FCGRT, RPS24, RPS18, GZMA</t>
-  </si>
-  <si>
-    <t>CCL5, GNB2L1, ATP5E, CD8B, HLA-B, TMEM66, CD1E, NKG7, RPL41, CD74</t>
-  </si>
-  <si>
-    <t>DNTT, MIR1244-2, GAS5, IL32, CD99, LTB, AC005912.1, NOP53, RPL34, SNHG29</t>
-  </si>
-  <si>
-    <t>SYN1, RNU6-540P, RP11-119D9.1, RPSAP15, PASK, HSPC324, AC010883.1, AC104563.1, AC096733.2, AP001059.3</t>
-  </si>
-  <si>
-    <t>GNB2L1, S100A4, HLA-B, RGS1, PTPRC, HLA-A, TSC22D3, GLTSCR2, SELM, RPS26</t>
-  </si>
-  <si>
-    <t>CCL5, KLRB1, DUSP2, GZMA, DNAJA4, RPL17, ANXA1, IGHA1, RPSAP15, DONSON</t>
-  </si>
-  <si>
-    <t>KLRB1, ANXA1, CEBPD, IL7R, IGHA1, ZNF683, RPLP1, RPSAP15, RPLP0, HLA-B</t>
+    <t>HBG2, HBA2, HLA-DQA2, HLA-DRB1, HLA-DRA, MALAT1, CD74, CD79A, HBA1, HSPA1B</t>
+  </si>
+  <si>
+    <t>MT-RNR2, IGHA1, JCHAIN, GAS5, RPL41, CD83, OR2A25, C11orf72, VPREB3, RP11-705C15.5</t>
+  </si>
+  <si>
+    <t>SOST, SERPINA9, GLYATL2, AICDA, REG1A, IFIT1B, LINC01644, BMP3, RP11-589C21.6, IL17A</t>
+  </si>
+  <si>
+    <t>RPS17, RACK1, CD74, MIR1244-2, HLA-DRA, IGKC, HES1, MT-ATP8, MT-ND3, IGHA2</t>
+  </si>
+  <si>
+    <t>TCL1A, IGHD, CD74, IGHM, YBX3, RPS17, IGKC, RPL41, RACK1, IL4R</t>
+  </si>
+  <si>
+    <t>MIR1244-2, GNG3, C11orf72, LINC01644, LINC02206, IFIT1B, OR2A25, GLYATL2, IGHV5-78, LINC01709</t>
+  </si>
+  <si>
+    <t>IGLL1, VPREB1, LINC01483, CMA1, LINC01644, RP11-589C21.6, CTAG2, ZFHX4-AS1, IL1RAPL1, GPIHBP1</t>
+  </si>
+  <si>
+    <t>CD79B, OR2A25, MIR1244-2, FCGR2C, IL22RA2, TLDC2, AICDA, CD207, IGHE, LINC02206</t>
+  </si>
+  <si>
+    <t>ZFHX4-AS1, VPREB1, FCGR2C, SIGLEC17P, RP11-84C10.2, LINC02202, C11orf72, HLA-DPB2, OR2A25, LINC01709</t>
+  </si>
+  <si>
+    <t>VPREB1, DNTT, XCR1, LINC01013, SOCS2-AS1, RP11-701P16.2, IGHE, RP11-84C10.2, RP11-589C21.6, OR2A25</t>
+  </si>
+  <si>
+    <t>IGHV5-78, RGS13, LINC01709, CD207, KIAA0087, C11orf72, GRIN1, OR2A25, LCNL1, LINC01644</t>
+  </si>
+  <si>
+    <t>SIGLEC17P, MMP12, TCL6, IGHE, IGHV5-78, SNHG26, AP001059.6, RP11-701P16.2, SNX29P1, DRAIC</t>
+  </si>
+  <si>
+    <t>OR2A25, DRAIC, LCNL1, C11orf72, FCGR2C, SYCP1, LINC01644, SIGLEC17P, LINC02202, PMCH</t>
+  </si>
+  <si>
+    <t>FCGR2C, RP11-589C21.6, AJ271736.10, IL22RA2, LINC02202, OR2A25, LINC01644, TCL1B, LDLRAD2, IL22</t>
+  </si>
+  <si>
+    <t>PCLAF, IGKC, KL, IGHV5-78, C11orf72, L3MBTL4-AS1, LINC01644, KIAA0087, GRIN1, IGHE</t>
+  </si>
+  <si>
+    <t>PCLAF, CD207, DUSP26, KIAA0087, IGHV5-78, CALB2, SOST, HLA-DPB2, SIGLEC17P, IL22RA2</t>
+  </si>
+  <si>
+    <t>RGS1, FCER1A, RP11-1275H24.3, LINC01644, SOCS2-AS1, OR2A25, IGHV5-78, SIGLEC17P, LCNL1, SYCP1</t>
+  </si>
+  <si>
+    <t>CLEC9A, WFDC21P, SYCP1, HLA-DPB2, FOXH1, RPS3AP34, OSTN-AS1, RP11-701P16.2, LINC01644, IL1RAPL1</t>
+  </si>
+  <si>
+    <t>CST3, RPL41, CLEC10A, JAML, HLA-DRB5, RPS17, HLA-DQB1, MMP9, IL22RA2, AGRP</t>
+  </si>
+  <si>
+    <t>FOXH1, FCN1, C11orf72, BMP3, GPIHBP1, LINC01644, FCER1A, OGDHL, LINC02206, OR2A25</t>
+  </si>
+  <si>
+    <t>BX255923.3, LINC01644, NCCRP1, IGHV5-78, ENTHD1, SIGLEC17P, WDR49, OR2A25, GPIHBP1, CIB3</t>
+  </si>
+  <si>
+    <t>SCT, FOXH1, SOST, SYCP1, HLA-DPB2, LINC01709, TCL1B, IGHE, RP11-1275H24.3, GPIHBP1</t>
+  </si>
+  <si>
+    <t>PCLAF, RNASE2, GPIHBP1, RPS3AP34, C11orf72, OGDHL, IGHE, SOCS2-AS1, RP11-589C21.6, LINC01644</t>
+  </si>
+  <si>
+    <t>CD99, IGLL1, PTCRA, FXYD2, PDLIM1, MFAP4, MZB1, JCHAIN, CD7, SELL</t>
+  </si>
+  <si>
+    <t>SMPD3, SH3TC1, ELOVL4, CD1B, CD8B, RP11-144L1.4, ARPP21, CD52, RAG2, CHRNA3</t>
+  </si>
+  <si>
+    <t>FOXH1, CCDC175, OR2A25, CIB3, AC098614.1, C11orf72, IGHV5-78, PCP2, IGHE, CD207</t>
+  </si>
+  <si>
+    <t>SELE, RAMP3, ACKR1, SOX17, ADGRL4, VWF, JAM2, MMRN2, SELP, RP11-536O18.1</t>
+  </si>
+  <si>
+    <t>ASCL1, PSMB11, FOXN1, WFDC2, PAX1, FOXG1, COL17A1, DSP, CDH3, TBATA</t>
+  </si>
+  <si>
+    <t>RP11-797H7.5, CTA-363E6.6, CTA-392E5.1, RP11-1275H24.3, LCNL1, LINC01644, IGHV5-78, ZNF812P, IL1RAPL1, GPIHBP1</t>
+  </si>
+  <si>
+    <t>FAM178B, APOC1, CD207, KIAA0087, PCLAF, OR2A25, LINC01644, PRSS57, IL17A, PRG2</t>
+  </si>
+  <si>
+    <t>IFIT1B, PMCH, OR2A25, LINC01644, SLC12A3, DRAIC, ABCC13, CTAG2, FOXH1, CD207</t>
+  </si>
+  <si>
+    <t>IGHE, AC098614.1, ZNF812P, LINC01644, XCR1, C11orf72, RP11-589C21.6, RPS3AP34, HOXB-AS3, IL17A</t>
+  </si>
+  <si>
+    <t>ACY3, LINC01644, WDR49, FOXH1, GPIHBP1, RP11-589C21.6, ZFHX4-AS1, KIAA0087, LINC01709, PENK</t>
+  </si>
+  <si>
+    <t>SMOC2, SFRP1, NTRK2, PRRX1, EBF2, OLFML1, MXRA5, F10, ANGPTL1, PDGFRA</t>
+  </si>
+  <si>
+    <t>SIGLEC17P, MS4A2, IGHV5-78, ZFHX4-AS1, RP11-589C21.6, OSTN-AS1, MAK, GPIHBP1, SLC10A5, KIAA0087</t>
+  </si>
+  <si>
+    <t>LINC01644, GATA3-AS1, OR2A25, TCL6, IL22RA2, IGHV5-78, SIGLEC17P, IGHE, LINC01709, FCGR2C</t>
+  </si>
+  <si>
+    <t>MPO, SIGLEC17P, SORD2P, AC098614.1, CD207, CPA3, SYCP1, ZFHX4-AS1, IL22, OR2A25</t>
+  </si>
+  <si>
+    <t>HBA2, HBG2, RACK1, ATP5F1E, HBA1, IGHV5-78, SIGLEC17P, SOST, ST18, RP11-505E24.2</t>
+  </si>
+  <si>
+    <t>IGHV5-78, MIR1-1HG-AS1, SIGLEC17P, GPIHBP1, LINC01644, REG1A, OSTN-AS1, KIAA0087, FOXH1, IGHE</t>
+  </si>
+  <si>
+    <t>FCGR2C, MPO, OR2A25, LINC02202, LINC02227, FOXP1-IT1, ZNF321P, LINC01943, OSTN-AS1, ELANE</t>
+  </si>
+  <si>
+    <t>AVP, SPINK2, ZNF321P, LINC01709, GATA3-AS1, DTX2P1-UPK3BP1-PMS2P11, OR2A25, CLEC9A, GRIN1, ERICH1-AS1</t>
+  </si>
+  <si>
+    <t>FCER1A, CKB, HBD, IGHE, DRAIC, HLA-DPB2, OR2A25, KIAA0087, C11orf72, ZFHX4-AS1</t>
+  </si>
+  <si>
+    <t>CTAG2, LINC01644, FOXH1, GIHCG, SIGLEC17P, RP11-701P16.2, LINC02206, IGHE, OR2A25, CALB2</t>
+  </si>
+  <si>
+    <t>MPO, MS4A3, LINC01709, OSTN-AS1, KIAA0087, KCNE5, CUX2, RP11-589C21.6, C11orf72, GPIHBP1</t>
+  </si>
+  <si>
+    <t>AREG, IL7R, IGHV5-78, XCR1, KLRB1, SYCP1, RP11-589C21.6, SIGLEC17P, LINC01644, GRIN1</t>
+  </si>
+  <si>
+    <t>SIGLEC17P, LINC01013, LINC01644, LINC02202, KIAA0087, SYCP1, OSTN-AS1, REG1A, IGHE, IL22</t>
+  </si>
+  <si>
+    <t>IGHE, IL17RB, LINC01709, MIR144, FCGR2C, TRDJ1, OR2A25, LINC02227, SNORA67, Metazoa_SRP</t>
+  </si>
+  <si>
+    <t>GATA3-AS1, FOXH1, EIF2S2P4, CD207, RP11-677O4.2, LINC02227, LINC01644, RP11-1275H24.3, SIGLEC17P, OSTN-AS1</t>
+  </si>
+  <si>
+    <t>FCER1G, GNLY, IGFBP7, TYROBP, GZMB, MYOM2, PTGDS, FCGR3A, PRSS57, ADAMTS1</t>
+  </si>
+  <si>
+    <t>TYROBP, LDB2, CCL3, FCER1G, NKG7, GSTP1, CLIC3, IRF8, CXCL3, KLRB1</t>
+  </si>
+  <si>
+    <t>NKG7, CST3, GNLY, SPINK2, HMOX1, MALAT1, IGFBP4, HBG2, STMN1, KLHL23</t>
+  </si>
+  <si>
+    <t>GNLY, TYROBP, KLRB1, PRDM16, FOXH1, AGRP, SYCP1, LINC02206, RP11-423H2.3, GPIHBP1</t>
+  </si>
+  <si>
+    <t>RBM24, GPIHBP1, IGHE, KIAA0087, HPN, PCDH9-AS1, HUNK, OR2A25, PDZK1, RP11-423H2.3</t>
+  </si>
+  <si>
+    <t>CGA, PAGE4, XAGE3, GAPLINC, PANX2, GATA3-AS1, LINC01644, LYVE1, ZFHX4-AS1, KIAA0087</t>
+  </si>
+  <si>
+    <t>IGHV5-78, LINC02206, KIAA0087, C11orf72, TCL1B, LINC01644, IGHE, FCGR2C, KLRF2, RP11-1275H24.3</t>
+  </si>
+  <si>
+    <t>TIMD4, CETP, SNORD3D, EGR2, PENK, LINC01644, ECSCR, ARRDC3, TCHH, CD5L</t>
+  </si>
+  <si>
+    <t>GNLY, APOE, C1QA, CD5L, FTL, FTH1, C1QB, APOC1, SELENOP, RNASE1</t>
+  </si>
+  <si>
+    <t>TPSAB1, CPA3, RP11-354E11.2, CMA1, IGHE, IL1RL1, SOST, CCNA1, KRT1, OR2A25</t>
+  </si>
+  <si>
+    <t>ADRA2A, PCDH9-AS1, FCER1A, OR2A25, SLC10A5, IL22, IGHV5-78, C11orf72, KIAA0087, RPL7P23</t>
+  </si>
+  <si>
+    <t>RP11-423H2.3, LY6G6F-LY6G6D, PF4V1, RP11-1275H24.3, SOST, LINC02227, OR2A25, GLYATL2, IGHV5-78, SDAD1P1</t>
+  </si>
+  <si>
+    <t>MTRNR2L10, IGHV5-78, LINC01644, TCL6, SOCS2-AS1, GATA3-AS1, LINC01483, IL17A, LINC01943, RPS3AP34</t>
+  </si>
+  <si>
+    <t>NKG7, KLRB1, HLA-DRA, KRT13, FTH1, SPRR3, C1QC, SAT1, LYZ, S100A2</t>
+  </si>
+  <si>
+    <t>RETN, RPS3AP34, LYZ, FCN1, LINC01644, IGHE, ST18, LCNL1, IGHV5-78, CUX2</t>
+  </si>
+  <si>
+    <t>S100A9, LINC02206, EEF1A1, CD207, TCL1B, CST7, OR2A25, SOST, IL22, MIR1-1HG-AS1</t>
+  </si>
+  <si>
+    <t>RHOC, HES4, MS4A7, DNAJA4, ABI3, BAG3, CUX2, IGHE, LINC02206, SIGLEC17P</t>
+  </si>
+  <si>
+    <t>TYROBP, FTL, IGKC, TRAC, RPS17, SAT1, NEAT1, LYZ, HLA-DPB1, IGLC2</t>
+  </si>
+  <si>
+    <t>LYZ, FTH1, MT-RNR2, S100A6, SRGN, FTL, TYROBP, ACTB, GPIHBP1, MT-ND3</t>
+  </si>
+  <si>
+    <t>SCT, FOXH1, LCNL1, SYCP1, OR2A25, LINC01709, DRAIC, TRIM71, OGDHL, LINC02227</t>
+  </si>
+  <si>
+    <t>MYBPH, DRAIC, LINC01709, SIGLEC17P, GPR15, REG1A, AGRP, IL22, C11orf72, SOST</t>
+  </si>
+  <si>
+    <t>JCHAIN, IGHA2, MZB1, XBP1, IGKC, RP11-354E11.2, RPL23AP18, TGFBR3L, C11orf72, ST18</t>
+  </si>
+  <si>
+    <t>PRTN3, ELANE, FCGR2C, AZU1, XCR1, LINC01644, LINC01709, FOXH1, CD207, GPIHBP1</t>
+  </si>
+  <si>
+    <t>NUCB2, CD27, LEF1, ZNF683, MALAT1, PRKCH, CD8A, GPIHBP1, TRGC2, CTSW</t>
+  </si>
+  <si>
+    <t>CD1E, ITM2A, MALAT1, SATB1, RPL10, CD44, FTL, TMSB10, RPS27, MT-ND2</t>
+  </si>
+  <si>
+    <t>KLRB1, SOCS3, CH25H, IGHV5-78, HOXB5, LINC01644, SIGLEC17P, GPIHBP1, ZFHX4-AS1, FOXH1</t>
+  </si>
+  <si>
+    <t>KIR2DL4, KLRC2, KCNK10, LINC02227, SYCP1, KIAA0087, GRIN1, ZFHX4-AS1, SIGLEC17P, LINC01644</t>
+  </si>
+  <si>
+    <t>KLRB1, IL7R, GZMK, LINC01709, CEBPD, LINC01871, KLRG1, IGHV5-78, BMP3, NCR3</t>
+  </si>
+  <si>
+    <t>GZMK, GZMA, SOST, IL22RA2, SIGLEC17P, IL26, RP11-84C10.2, PENK, PPP3CB-AS1, MIR144</t>
+  </si>
+  <si>
+    <t>NKG7, GNLY, IL32, PRDM16, ITM2C, LINC02227, CD52, RPS3AP34, TCL1B, FOXH1</t>
+  </si>
+  <si>
+    <t>MS4A6A, IL32, TIMD4, PTPRCAP, RTKN2, TIGIT, MIR4435-2HG, RGS1, SRGN, FOXH1</t>
+  </si>
+  <si>
+    <t>HLA-B, CD74, SMS, COTL1, PTPRC, TUBB, BIRC3, B2M, ITM2A, HLA-A</t>
+  </si>
+  <si>
+    <t>CD8B, CD8A, LINC02446, B2M, FTL, HLA-C, RPS2, GAS5, HLA-A, HLA-B</t>
+  </si>
+  <si>
+    <t>IGFBP1, MT-RNR2, FCGRT, TMSB10, SNHG3, HBG1, RPS18, LTB, LINC01709, CTSL</t>
+  </si>
+  <si>
+    <t>CCL5, CD8B, CD8A, GZMK, RPS29, RPS2, ATP5F1E, CST7, IGHM, NKG7</t>
+  </si>
+  <si>
+    <t>GZMH, RP11-466H18.1, FCGR2C, SIGLEC17P, PZP, IL7R, OR2A25, MT-ND3, RP11-1275H24.3, SNX29P1</t>
+  </si>
+  <si>
+    <t>CCL5, CD8A, IGHA1, CCL4, RPLP2, IFIT1B, CD8B, IGHV5-78, IL7R, LINC01644</t>
+  </si>
+  <si>
+    <t>ANXA1, DNTT, MIR1244-2, KLRB1, S100A4, DONSON, AQP3, LTB, RP11-589C21.6, SFTPA1</t>
+  </si>
+  <si>
+    <t>FOXH1, RP11-589C21.6, SOST, CTAG2, PANX2, IGHV5-78, ZFHX4-AS1, SOCS2-AS1, KIAA0087, INPP5J</t>
+  </si>
+  <si>
+    <t>S100A4, HLA-B, RPS26, RGS1, HLA-A, CD1E, TSC22D3, PTPRC, FCGR2C, SIGLEC17P</t>
+  </si>
+  <si>
+    <t>CCL5, KLRB1, SIGLEC17P, FCGR2C, RPL17, CEBPB, PRDM16, ANXA1, FOXH1, TCL1B</t>
+  </si>
+  <si>
+    <t>KLRB1, ANXA1, S100A4, CEBPD, FCGR2C, MIR144, IGHE, LINC02245, LINC02206, LINC02202</t>
   </si>
 </sst>
 </file>
@@ -2060,7 +2066,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H92"/>
+  <dimension ref="A1:H91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2103,19 +2109,19 @@
         <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F2" t="s">
         <v>322</v>
       </c>
       <c r="G2" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="H2" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2129,19 +2135,19 @@
         <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F3" t="s">
         <v>323</v>
       </c>
       <c r="G3" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="H3" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2155,19 +2161,19 @@
         <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F4" t="s">
         <v>324</v>
       </c>
       <c r="G4" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="H4" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2181,19 +2187,19 @@
         <v>105</v>
       </c>
       <c r="D5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F5" t="s">
         <v>325</v>
       </c>
       <c r="G5" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="H5" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2207,19 +2213,19 @@
         <v>106</v>
       </c>
       <c r="D6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E6" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F6" t="s">
         <v>326</v>
       </c>
       <c r="G6" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="H6" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2233,19 +2239,19 @@
         <v>107</v>
       </c>
       <c r="D7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F7" t="s">
         <v>327</v>
       </c>
       <c r="G7" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="H7" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2259,19 +2265,19 @@
         <v>108</v>
       </c>
       <c r="D8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E8" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F8" t="s">
         <v>328</v>
       </c>
       <c r="G8" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="H8" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2285,19 +2291,19 @@
         <v>109</v>
       </c>
       <c r="D9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G9" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="H9" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2311,19 +2317,19 @@
         <v>110</v>
       </c>
       <c r="D10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F10" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="G10" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="H10" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2337,7 +2343,7 @@
         <v>111</v>
       </c>
       <c r="D11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E11" t="s">
         <v>267</v>
@@ -2346,10 +2352,10 @@
         <v>328</v>
       </c>
       <c r="G11" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="H11" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2363,19 +2369,19 @@
         <v>112</v>
       </c>
       <c r="D12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E12" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="F12" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G12" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="H12" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2389,19 +2395,19 @@
         <v>113</v>
       </c>
       <c r="D13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E13" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="F13" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G13" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="H13" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2415,19 +2421,19 @@
         <v>114</v>
       </c>
       <c r="D14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E14" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="F14" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G14" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="H14" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2441,19 +2447,19 @@
         <v>115</v>
       </c>
       <c r="D15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E15" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="F15" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="G15" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="H15" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2467,19 +2473,19 @@
         <v>116</v>
       </c>
       <c r="D16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F16" t="s">
         <v>333</v>
       </c>
       <c r="G16" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="H16" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2493,19 +2499,19 @@
         <v>117</v>
       </c>
       <c r="D17" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E17" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F17" t="s">
         <v>334</v>
       </c>
       <c r="G17" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="H17" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2519,19 +2525,19 @@
         <v>118</v>
       </c>
       <c r="D18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E18" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F18" t="s">
         <v>335</v>
       </c>
       <c r="G18" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="H18" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2545,19 +2551,19 @@
         <v>119</v>
       </c>
       <c r="D19" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E19" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F19" t="s">
         <v>336</v>
       </c>
       <c r="G19" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="H19" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2571,19 +2577,19 @@
         <v>120</v>
       </c>
       <c r="D20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E20" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F20" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G20" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="H20" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2597,19 +2603,19 @@
         <v>121</v>
       </c>
       <c r="D21" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E21" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="F21" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="G21" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="H21" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2623,19 +2629,19 @@
         <v>122</v>
       </c>
       <c r="D22" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E22" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F22" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="G22" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="H22" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2649,19 +2655,19 @@
         <v>123</v>
       </c>
       <c r="D23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E23" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="F23" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="G23" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="H23" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2675,19 +2681,19 @@
         <v>124</v>
       </c>
       <c r="D24" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E24" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F24" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="G24" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="H24" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2701,19 +2707,19 @@
         <v>125</v>
       </c>
       <c r="D25" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E25" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="F25" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="G25" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="H25" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2727,19 +2733,19 @@
         <v>126</v>
       </c>
       <c r="D26" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E26" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F26" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G26" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="H26" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2753,19 +2759,19 @@
         <v>127</v>
       </c>
       <c r="D27" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E27" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="F27" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="G27" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="H27" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2779,19 +2785,19 @@
         <v>128</v>
       </c>
       <c r="D28" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F28" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="G28" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="H28" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2805,19 +2811,19 @@
         <v>129</v>
       </c>
       <c r="D29" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E29" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F29" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G29" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="H29" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2831,19 +2837,19 @@
         <v>130</v>
       </c>
       <c r="D30" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E30" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F30" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="G30" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="H30" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2857,19 +2863,19 @@
         <v>131</v>
       </c>
       <c r="D31" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E31" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F31" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="G31" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="H31" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2883,19 +2889,19 @@
         <v>132</v>
       </c>
       <c r="D32" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E32" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="F32" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="G32" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="H32" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2909,19 +2915,19 @@
         <v>133</v>
       </c>
       <c r="D33" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E33" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="F33" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G33" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="H33" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2935,19 +2941,19 @@
         <v>134</v>
       </c>
       <c r="D34" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E34" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="F34" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="G34" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="H34" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2961,19 +2967,19 @@
         <v>135</v>
       </c>
       <c r="D35" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E35" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="F35" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="G35" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="H35" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2987,19 +2993,19 @@
         <v>136</v>
       </c>
       <c r="D36" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E36" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F36" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="G36" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="H36" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -3013,19 +3019,19 @@
         <v>137</v>
       </c>
       <c r="D37" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E37" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="F37" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="G37" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="H37" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -3039,19 +3045,19 @@
         <v>138</v>
       </c>
       <c r="D38" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E38" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="F38" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="G38" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="H38" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -3065,19 +3071,19 @@
         <v>139</v>
       </c>
       <c r="D39" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E39" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F39" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="G39" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="H39" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -3091,19 +3097,19 @@
         <v>140</v>
       </c>
       <c r="D40" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E40" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F40" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="G40" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="H40" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -3117,19 +3123,19 @@
         <v>141</v>
       </c>
       <c r="D41" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E41" t="s">
-        <v>266</v>
+        <v>284</v>
       </c>
       <c r="F41" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="G41" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="H41" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -3143,19 +3149,19 @@
         <v>142</v>
       </c>
       <c r="D42" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E42" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="F42" t="s">
-        <v>328</v>
+        <v>350</v>
       </c>
       <c r="G42" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="H42" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -3169,19 +3175,19 @@
         <v>143</v>
       </c>
       <c r="D43" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E43" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F43" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="G43" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="H43" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -3195,19 +3201,19 @@
         <v>144</v>
       </c>
       <c r="D44" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E44" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="F44" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="G44" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="H44" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -3221,19 +3227,19 @@
         <v>145</v>
       </c>
       <c r="D45" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E45" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F45" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G45" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="H45" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -3247,19 +3253,19 @@
         <v>146</v>
       </c>
       <c r="D46" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E46" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F46" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="G46" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="H46" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -3273,19 +3279,19 @@
         <v>147</v>
       </c>
       <c r="D47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E47" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F47" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="G47" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="H47" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -3299,19 +3305,19 @@
         <v>148</v>
       </c>
       <c r="D48" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E48" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F48" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="G48" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="H48" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -3325,19 +3331,19 @@
         <v>149</v>
       </c>
       <c r="D49" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E49" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F49" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G49" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="H49" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -3351,19 +3357,19 @@
         <v>150</v>
       </c>
       <c r="D50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E50" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F50" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G50" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="H50" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -3377,19 +3383,19 @@
         <v>151</v>
       </c>
       <c r="D51" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E51" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F51" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="G51" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="H51" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -3403,19 +3409,19 @@
         <v>152</v>
       </c>
       <c r="D52" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E52" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F52" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="G52" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="H52" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -3429,19 +3435,19 @@
         <v>153</v>
       </c>
       <c r="D53" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E53" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F53" t="s">
-        <v>355</v>
+        <v>327</v>
       </c>
       <c r="G53" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="H53" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -3455,19 +3461,19 @@
         <v>154</v>
       </c>
       <c r="D54" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E54" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
       <c r="F54" t="s">
-        <v>348</v>
+        <v>330</v>
       </c>
       <c r="G54" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="H54" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -3481,19 +3487,19 @@
         <v>155</v>
       </c>
       <c r="D55" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E55" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F55" t="s">
-        <v>345</v>
+        <v>358</v>
       </c>
       <c r="G55" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="H55" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -3507,19 +3513,19 @@
         <v>156</v>
       </c>
       <c r="D56" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E56" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F56" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="G56" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="H56" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -3533,19 +3539,19 @@
         <v>157</v>
       </c>
       <c r="D57" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E57" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F57" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="G57" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="H57" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -3559,19 +3565,19 @@
         <v>158</v>
       </c>
       <c r="D58" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E58" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F58" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="G58" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="H58" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -3585,19 +3591,19 @@
         <v>159</v>
       </c>
       <c r="D59" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E59" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F59" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="G59" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="H59" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -3611,19 +3617,19 @@
         <v>160</v>
       </c>
       <c r="D60" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E60" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="F60" t="s">
-        <v>327</v>
+        <v>348</v>
       </c>
       <c r="G60" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="H60" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -3637,19 +3643,19 @@
         <v>161</v>
       </c>
       <c r="D61" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E61" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="F61" t="s">
-        <v>328</v>
+        <v>340</v>
       </c>
       <c r="G61" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="H61" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -3663,19 +3669,19 @@
         <v>162</v>
       </c>
       <c r="D62" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E62" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F62" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="G62" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="H62" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -3689,19 +3695,19 @@
         <v>163</v>
       </c>
       <c r="D63" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E63" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F63" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="G63" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="H63" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -3715,19 +3721,19 @@
         <v>164</v>
       </c>
       <c r="D64" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E64" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="F64" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="G64" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="H64" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -3741,19 +3747,19 @@
         <v>165</v>
       </c>
       <c r="D65" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E65" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F65" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="G65" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="H65" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -3767,19 +3773,19 @@
         <v>166</v>
       </c>
       <c r="D66" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E66" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F66" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="G66" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="H66" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -3793,19 +3799,19 @@
         <v>167</v>
       </c>
       <c r="D67" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E67" t="s">
         <v>301</v>
       </c>
       <c r="F67" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="G67" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="H67" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -3819,19 +3825,19 @@
         <v>168</v>
       </c>
       <c r="D68" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E68" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="F68" t="s">
-        <v>355</v>
+        <v>366</v>
       </c>
       <c r="G68" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="H68" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -3845,19 +3851,19 @@
         <v>169</v>
       </c>
       <c r="D69" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E69" t="s">
         <v>303</v>
       </c>
       <c r="F69" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="G69" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="H69" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3871,19 +3877,19 @@
         <v>170</v>
       </c>
       <c r="D70" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E70" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F70" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="G70" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="H70" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -3897,19 +3903,19 @@
         <v>171</v>
       </c>
       <c r="D71" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E71" t="s">
         <v>304</v>
       </c>
       <c r="F71" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="G71" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="H71" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -3923,19 +3929,19 @@
         <v>172</v>
       </c>
       <c r="D72" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E72" t="s">
-        <v>266</v>
+        <v>284</v>
       </c>
       <c r="F72" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="G72" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="H72" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3949,19 +3955,19 @@
         <v>173</v>
       </c>
       <c r="D73" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E73" t="s">
         <v>305</v>
       </c>
       <c r="F73" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="G73" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="H73" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -3975,19 +3981,19 @@
         <v>174</v>
       </c>
       <c r="D74" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E74" t="s">
-        <v>277</v>
+        <v>306</v>
       </c>
       <c r="F74" t="s">
-        <v>339</v>
+        <v>370</v>
       </c>
       <c r="G74" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="H74" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -4001,19 +4007,19 @@
         <v>175</v>
       </c>
       <c r="D75" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E75" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F75" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="G75" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="H75" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -4027,19 +4033,19 @@
         <v>176</v>
       </c>
       <c r="D76" t="s">
-        <v>249</v>
+        <v>202</v>
       </c>
       <c r="E76" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F76" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="G76" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="H76" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -4053,19 +4059,19 @@
         <v>177</v>
       </c>
       <c r="D77" t="s">
-        <v>204</v>
+        <v>247</v>
       </c>
       <c r="E77" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F77" t="s">
-        <v>331</v>
+        <v>373</v>
       </c>
       <c r="G77" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="H77" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -4079,19 +4085,19 @@
         <v>178</v>
       </c>
       <c r="D78" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E78" t="s">
-        <v>309</v>
+        <v>280</v>
       </c>
       <c r="F78" t="s">
-        <v>368</v>
+        <v>346</v>
       </c>
       <c r="G78" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="H78" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -4105,19 +4111,19 @@
         <v>179</v>
       </c>
       <c r="D79" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E79" t="s">
         <v>310</v>
       </c>
       <c r="F79" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="G79" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="H79" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -4131,19 +4137,19 @@
         <v>180</v>
       </c>
       <c r="D80" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E80" t="s">
-        <v>277</v>
+        <v>311</v>
       </c>
       <c r="F80" t="s">
-        <v>339</v>
+        <v>375</v>
       </c>
       <c r="G80" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="H80" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -4157,19 +4163,19 @@
         <v>181</v>
       </c>
       <c r="D81" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E81" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F81" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="G81" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="H81" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -4183,19 +4189,19 @@
         <v>182</v>
       </c>
       <c r="D82" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E82" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F82" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="G82" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="H82" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -4203,25 +4209,25 @@
         <v>39</v>
       </c>
       <c r="B83" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="C83" t="s">
         <v>183</v>
       </c>
       <c r="D83" t="s">
-        <v>207</v>
+        <v>252</v>
       </c>
       <c r="E83" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F83" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="G83" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="H83" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -4229,25 +4235,25 @@
         <v>39</v>
       </c>
       <c r="B84" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C84" t="s">
         <v>184</v>
       </c>
       <c r="D84" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E84" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F84" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="G84" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="H84" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -4255,25 +4261,25 @@
         <v>39</v>
       </c>
       <c r="B85" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C85" t="s">
         <v>185</v>
       </c>
       <c r="D85" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E85" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="F85" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="G85" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="H85" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -4281,25 +4287,25 @@
         <v>39</v>
       </c>
       <c r="B86" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C86" t="s">
         <v>186</v>
       </c>
       <c r="D86" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E86" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F86" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="G86" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="H86" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -4307,25 +4313,25 @@
         <v>39</v>
       </c>
       <c r="B87" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C87" t="s">
         <v>187</v>
       </c>
       <c r="D87" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E87" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F87" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="G87" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="H87" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -4333,25 +4339,25 @@
         <v>39</v>
       </c>
       <c r="B88" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C88" t="s">
         <v>188</v>
       </c>
       <c r="D88" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E88" t="s">
-        <v>318</v>
+        <v>280</v>
       </c>
       <c r="F88" t="s">
-        <v>377</v>
+        <v>346</v>
       </c>
       <c r="G88" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="H88" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -4359,25 +4365,25 @@
         <v>39</v>
       </c>
       <c r="B89" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C89" t="s">
         <v>189</v>
       </c>
       <c r="D89" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="E89" t="s">
-        <v>277</v>
+        <v>319</v>
       </c>
       <c r="F89" t="s">
-        <v>339</v>
+        <v>382</v>
       </c>
       <c r="G89" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="H89" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -4385,25 +4391,25 @@
         <v>39</v>
       </c>
       <c r="B90" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C90" t="s">
         <v>190</v>
       </c>
       <c r="D90" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E90" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F90" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="G90" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="H90" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -4411,51 +4417,25 @@
         <v>39</v>
       </c>
       <c r="B91" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C91" t="s">
         <v>191</v>
       </c>
       <c r="D91" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E91" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F91" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="G91" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="H91" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
-      <c r="A92" t="s">
-        <v>39</v>
-      </c>
-      <c r="B92" t="s">
-        <v>101</v>
-      </c>
-      <c r="C92" t="s">
-        <v>192</v>
-      </c>
-      <c r="D92" t="s">
-        <v>260</v>
-      </c>
-      <c r="E92" t="s">
-        <v>321</v>
-      </c>
-      <c r="F92" t="s">
-        <v>380</v>
-      </c>
-      <c r="G92" t="s">
-        <v>471</v>
-      </c>
-      <c r="H92" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>